<commit_message>
added data for latest run 4621
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_H.BROWN_06.18.20.xlsx
+++ b/bioSample/bioSample_H.BROWN_06.18.20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648C9CF9-655D-C348-8B38-BB2C373C6EB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A34648F-912D-DA49-A462-1E6174DED252}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25860" windowHeight="12300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,7 +456,7 @@
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="23.83203125" customWidth="1"/>
     <col min="5" max="5" width="21.1640625" customWidth="1"/>
-    <col min="6" max="6" width="6" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
     <col min="7" max="7" width="12.5" customWidth="1"/>
     <col min="8" max="8" width="16.5" customWidth="1"/>
     <col min="9" max="9" width="9.1640625" customWidth="1"/>

</xml_diff>